<commit_message>
Function Point Calculation and Time Estimation
Semester 2 HW 3 - Unfinished
</commit_message>
<xml_diff>
--- a/Use Case/UCTimeLog.xlsx
+++ b/Use Case/UCTimeLog.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
   <si>
     <t>UC</t>
   </si>
@@ -63,6 +63,24 @@
   </si>
   <si>
     <t>Edit personal Data</t>
+  </si>
+  <si>
+    <t>Semester 3:</t>
+  </si>
+  <si>
+    <t>Semester 4:</t>
+  </si>
+  <si>
+    <t>Bet on Win</t>
+  </si>
+  <si>
+    <t>Buy Reward</t>
+  </si>
+  <si>
+    <t>Check Game Results</t>
+  </si>
+  <si>
+    <t>Estimated:</t>
   </si>
 </sst>
 </file>
@@ -112,7 +130,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -121,6 +139,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -138,6 +159,1110 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="de-DE"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t>FP calculation</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-GB" baseline="0"/>
+              <a:t> and time estimation</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-GB"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+                <a:prstDash val="solid"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:forward val="2"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout/>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>UC!$E$5:$E$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>3.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>9.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>UC!$F$5:$F$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>15.3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>17.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>14.9</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>49.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>39.6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>30.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="192860048"/>
+        <c:axId val="192859264"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="192860048"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Hours</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB" baseline="0"/>
+                  <a:t> spent</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="192859264"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="192859264"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="80"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Function Points</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="192860048"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.7" r="0.7" t="0.78740157499999996" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>742950</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>14286</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>742950</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>47624</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Diagramm 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -403,10 +1528,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A2:F16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -420,154 +1545,244 @@
     <col min="7" max="16384" width="11.42578125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" s="2">
-        <v>1</v>
-      </c>
-      <c r="C2" s="2">
-        <v>2</v>
-      </c>
-      <c r="D2" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="E2" s="3">
-        <f>SUM(B2,C2,D2)</f>
-        <v>3.5</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" s="2">
-        <v>1.5</v>
-      </c>
-      <c r="C3" s="2">
-        <v>4</v>
-      </c>
-      <c r="D3" s="2">
-        <v>1</v>
-      </c>
-      <c r="E3" s="3">
-        <f t="shared" ref="E3:E8" si="0">SUM(B3,C3,D3)</f>
-        <v>6.5</v>
-      </c>
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" s="2">
-        <v>1</v>
-      </c>
-      <c r="C4" s="2">
-        <v>6.5</v>
-      </c>
-      <c r="D4" s="2">
-        <v>2</v>
-      </c>
-      <c r="E4" s="3">
-        <f t="shared" si="0"/>
-        <v>9.5</v>
-      </c>
+    <row r="4" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B5" s="2">
-        <v>1.5</v>
+        <v>1</v>
       </c>
       <c r="C5" s="2">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D5" s="2">
         <v>0.5</v>
       </c>
       <c r="E5" s="3">
-        <f t="shared" si="0"/>
-        <v>6</v>
+        <f>SUM(B5,C5,D5)</f>
+        <v>3.5</v>
+      </c>
+      <c r="F5" s="2">
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B6" s="2">
-        <v>1.5</v>
+        <v>1</v>
       </c>
       <c r="C6" s="2">
-        <v>3</v>
+        <v>2.5</v>
       </c>
       <c r="D6" s="2">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="E6" s="3">
-        <f t="shared" si="0"/>
-        <v>5.5</v>
+        <f>SUM(B6,C6,D6)</f>
+        <v>4</v>
+      </c>
+      <c r="F6" s="2">
+        <v>15.3</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B7" s="2">
+        <v>1.5</v>
+      </c>
+      <c r="C7" s="2">
+        <v>3</v>
+      </c>
+      <c r="D7" s="2">
         <v>1</v>
       </c>
-      <c r="C7" s="2">
-        <v>2.5</v>
-      </c>
-      <c r="D7" s="2">
-        <v>0.5</v>
-      </c>
       <c r="E7" s="3">
-        <f t="shared" si="0"/>
-        <v>4</v>
+        <f>SUM(B7,C7,D7)</f>
+        <v>5.5</v>
+      </c>
+      <c r="F7" s="2">
+        <v>17.5</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="2">
+        <v>1.5</v>
+      </c>
+      <c r="C8" s="2">
+        <v>4</v>
+      </c>
+      <c r="D8" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="E8" s="3">
+        <f>SUM(B8,C8,D8)</f>
+        <v>6</v>
+      </c>
+      <c r="F8" s="2">
+        <v>14.9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="2">
+        <v>1.5</v>
+      </c>
+      <c r="C9" s="2">
+        <v>4</v>
+      </c>
+      <c r="D9" s="2">
+        <v>1</v>
+      </c>
+      <c r="E9" s="3">
+        <f>SUM(B9,C9,D9)</f>
+        <v>6.5</v>
+      </c>
+      <c r="F9" s="2">
+        <v>49.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="2">
+      <c r="B10" s="2">
         <v>1</v>
       </c>
-      <c r="C8" s="2">
+      <c r="C10" s="2">
         <v>4.5</v>
       </c>
-      <c r="D8" s="2">
+      <c r="D10" s="2">
         <v>1.5</v>
       </c>
-      <c r="E8" s="3">
+      <c r="E10" s="3">
+        <f>SUM(B10,C10,D10)</f>
+        <v>7</v>
+      </c>
+      <c r="F10" s="2">
+        <v>39.6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" s="2">
+        <v>1</v>
+      </c>
+      <c r="C11" s="2">
+        <v>6.5</v>
+      </c>
+      <c r="D11" s="2">
+        <v>2</v>
+      </c>
+      <c r="E11" s="3">
+        <f>SUM(B11,C11,D11)</f>
+        <v>9.5</v>
+      </c>
+      <c r="F11" s="2">
+        <v>30.5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E14" s="2">
+        <f>(F14-4.7839)/3.6146</f>
+        <v>5.1502517567642343</v>
+      </c>
+      <c r="F14" s="2">
+        <v>23.4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E15" s="2">
+        <f t="shared" ref="E15:E16" si="0">(F15-4.7839)/3.6146</f>
+        <v>5.1502517567642343</v>
+      </c>
+      <c r="F15" s="2">
+        <v>23.4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E16" s="2">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>21.334615171803243</v>
+      </c>
+      <c r="F16" s="2">
+        <v>81.900000000000006</v>
       </c>
     </row>
   </sheetData>
+  <sortState ref="A5:F11">
+    <sortCondition ref="E5:E11"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
UCTimeLog add predictions to FP table
</commit_message>
<xml_diff>
--- a/Use Case/UCTimeLog.xlsx
+++ b/Use Case/UCTimeLog.xlsx
@@ -378,6 +378,77 @@
             </c:ext>
           </c:extLst>
         </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Predictions</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>UC!$E$14:$E$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>5.1502517567642343</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.1502517567642343</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>21.334615171803243</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>UC!$F$14:$F$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>23.4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>23.4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>81.900000000000006</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-9C6F-49AB-960D-9254F3D89603}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
@@ -514,7 +585,6 @@
         <c:axId val="192859264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="80"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -1563,8 +1633,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:F16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView tabSelected="1" topLeftCell="C4" workbookViewId="0">
+      <selection activeCell="R12" sqref="R12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>